<commit_message>
Base de datos Colombia
</commit_message>
<xml_diff>
--- a/Indicadores Colombia.xlsx
+++ b/Indicadores Colombia.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan David\Documents\Python\Bootcamp_project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61F31F38-36F0-4956-BD59-2C0983351251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AB198F-84E8-4776-A235-D80A6A78CC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{30DEC2AF-C895-466C-8EA5-CE5386A1C26E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{30DEC2AF-C895-466C-8EA5-CE5386A1C26E}"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="1" r:id="rId1"/>
     <sheet name="Desempleo" sheetId="2" r:id="rId2"/>
     <sheet name="Inflacion" sheetId="4" r:id="rId3"/>
-    <sheet name="Tasas_de_interes" sheetId="5" r:id="rId4"/>
+    <sheet name="Tasa_de_interes" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,9 +41,6 @@
     <t>PIB</t>
   </si>
   <si>
-    <t>Delta PIB</t>
-  </si>
-  <si>
     <t>Exportaciones</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
   </si>
   <si>
     <t>Delta_Desoc</t>
-  </si>
-  <si>
-    <t>Meta inflación</t>
   </si>
   <si>
     <t>Inflacion</t>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>TES7</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Delta_PIB</t>
   </si>
 </sst>
 </file>
@@ -446,24 +446,6 @@
   </cellStyles>
   <dxfs count="52">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -786,13 +768,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -826,6 +801,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1180,6 +1162,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1188,22 +1186,6 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1212,32 +1194,13 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1580,29 +1543,54 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1611,12 +1599,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2035,13 +2017,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2082,6 +2057,31 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2096,69 +2096,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00C3610B-2979-4915-BC8B-6079C7085CAF}" name="Tabla1" displayName="Tabla1" ref="A1:I17" totalsRowShown="0" headerRowDxfId="38" dataDxfId="51" headerRowBorderDxfId="49" tableBorderDxfId="50" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00C3610B-2979-4915-BC8B-6079C7085CAF}" name="Tabla1" displayName="Tabla1" ref="A1:I17" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
   <autoFilter ref="A1:I17" xr:uid="{00C3610B-2979-4915-BC8B-6079C7085CAF}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{4140CAED-D83F-4605-A3C9-3B410DE1A5D2}" name="Periodo" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{BB556350-3E93-4F4A-9AFC-4033BEFF3C21}" name="PIB" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{A5D0D2AE-AFDE-4791-A435-566372823042}" name="Delta PIB" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{B798777A-D692-4782-9A67-F3C970CD959C}" name="Formacion_Capital" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{8221F72B-08C3-49FE-8C73-9CDDB012C518}" name="Delta_Formacion" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{E0067DB4-0B66-4E56-AC60-65AA1BE2F25D}" name="Exportaciones" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{6DEB60BA-1D24-4B7E-8421-ED3AD1E6D1C4}" name="Delta_Expo" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{43E6BB03-0733-439A-ABEC-3E625BC4C794}" name="Importaciones" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{9C7EBC4F-D5C6-4352-874D-7FA165FD0DBA}" name="Delta_Import" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{4140CAED-D83F-4605-A3C9-3B410DE1A5D2}" name="Periodo" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{BB556350-3E93-4F4A-9AFC-4033BEFF3C21}" name="PIB" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{A5D0D2AE-AFDE-4791-A435-566372823042}" name="Delta_PIB" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{B798777A-D692-4782-9A67-F3C970CD959C}" name="Formacion_Capital" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{8221F72B-08C3-49FE-8C73-9CDDB012C518}" name="Delta_Formacion" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{E0067DB4-0B66-4E56-AC60-65AA1BE2F25D}" name="Exportaciones" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{6DEB60BA-1D24-4B7E-8421-ED3AD1E6D1C4}" name="Delta_Expo" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{43E6BB03-0733-439A-ABEC-3E625BC4C794}" name="Importaciones" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{9C7EBC4F-D5C6-4352-874D-7FA165FD0DBA}" name="Delta_Import" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{747B7C06-C17D-4ACF-B377-C80F82C8BBEF}" name="Tabla2" displayName="Tabla2" ref="A1:H22" totalsRowShown="0" headerRowDxfId="25" dataDxfId="26" headerRowBorderDxfId="36" tableBorderDxfId="37" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{747B7C06-C17D-4ACF-B377-C80F82C8BBEF}" name="Tabla2" displayName="Tabla2" ref="A1:H22" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A1:H22" xr:uid="{747B7C06-C17D-4ACF-B377-C80F82C8BBEF}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8E303D79-9181-4B3F-9CE6-5EDAE53EAC47}" name="Periodo" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{938D8137-D063-445B-A2FA-048FA4428BD0}" name="Poblacion" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{5B393CA8-5E73-4377-933F-53ABED706BBC}" name="PET" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{DDB8A59F-F18B-4B98-B616-E0F4C93BE404}" name="Delta_PET" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{9AC913E9-52E0-4FB1-8737-DB9A11F5CCC3}" name="PEA" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{A4F4E0A4-31B4-4AB7-9742-13AB761B78FE}" name="Delta_PEA" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{544ADB02-B2A6-4549-9A59-B0450D058EDF}" name="Desocupados" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{F7F9AD16-917D-4D00-B04E-893B87223637}" name="Delta_Desoc" dataDxfId="27" dataCellStyle="Porcentaje"/>
+    <tableColumn id="1" xr3:uid="{8E303D79-9181-4B3F-9CE6-5EDAE53EAC47}" name="Periodo" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{938D8137-D063-445B-A2FA-048FA4428BD0}" name="Poblacion" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{5B393CA8-5E73-4377-933F-53ABED706BBC}" name="PET" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{DDB8A59F-F18B-4B98-B616-E0F4C93BE404}" name="Delta_PET" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{9AC913E9-52E0-4FB1-8737-DB9A11F5CCC3}" name="PEA" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{A4F4E0A4-31B4-4AB7-9742-13AB761B78FE}" name="Delta_PEA" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{544ADB02-B2A6-4549-9A59-B0450D058EDF}" name="Desocupados" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{F7F9AD16-917D-4D00-B04E-893B87223637}" name="Delta_Desoc" dataDxfId="25" dataCellStyle="Porcentaje"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D494C66-0C85-4D48-87FA-B022B18C9539}" name="Tabla3" displayName="Tabla3" ref="A1:H23" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="23" tableBorderDxfId="24" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D494C66-0C85-4D48-87FA-B022B18C9539}" name="Tabla3" displayName="Tabla3" ref="A1:H23" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A1:H23" xr:uid="{7D494C66-0C85-4D48-87FA-B022B18C9539}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E4D64D60-EC06-4251-9D19-C95099CE1CEC}" name="Periodo" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{3E632234-5948-424D-89E9-12C5F0B5FE39}" name="Meta inflación" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{E8169260-7D6F-4E40-9C5A-67FB5E86C22B}" name="Inflacion" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C3E4F19F-EAEC-42EE-9434-FCF4B0ED0B12}" name="Inflacion_a" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{8C47B3DF-6DF9-4374-9038-23702C9A126B}" name="Inflacion_p" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{994B10DA-E399-41E2-AA69-D63844110D53}" name="TRM" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{FDD56685-3044-4C36-95B7-3630E5D0A95F}" name="Dev_nom" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{9B184471-DE19-4E9C-B4ED-A14E0D69A061}" name="Dev_real" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{E4D64D60-EC06-4251-9D19-C95099CE1CEC}" name="Periodo" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{3E632234-5948-424D-89E9-12C5F0B5FE39}" name="Meta" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{E8169260-7D6F-4E40-9C5A-67FB5E86C22B}" name="Inflacion" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{C3E4F19F-EAEC-42EE-9434-FCF4B0ED0B12}" name="Inflacion_a" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{8C47B3DF-6DF9-4374-9038-23702C9A126B}" name="Inflacion_p" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{994B10DA-E399-41E2-AA69-D63844110D53}" name="TRM" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{FDD56685-3044-4C36-95B7-3630E5D0A95F}" name="Dev_nom" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{9B184471-DE19-4E9C-B4ED-A14E0D69A061}" name="Dev_real" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C0BE5DF4-6E68-4AA6-85BD-FA91069871B5}" name="Tabla4" displayName="Tabla4" ref="A1:H23" totalsRowShown="0" headerRowDxfId="0" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C0BE5DF4-6E68-4AA6-85BD-FA91069871B5}" name="Tabla4" displayName="Tabla4" ref="A1:H23" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H23" xr:uid="{C0BE5DF4-6E68-4AA6-85BD-FA91069871B5}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BDF4F3C4-0105-422C-89EC-1C044F17D164}" name="Periodo" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CD18CA5F-849B-477D-8347-AEC7C9F9C1A3}" name="Tasa_inter" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{7498D1B7-EF61-4ABC-A39A-C1ED050FE05F}" name="Consumo" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{5D1D2915-40B4-4440-B8E5-EC65A8C1BDE2}" name="Comercial" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{B3A56FF1-A864-41BA-9CEB-83FCFDC4BA73}" name="Hipotecario" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{40E2355E-A7FB-42F5-AF3D-31DBC2503E8C}" name="TES1" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{AE326550-1A7E-40C8-856D-05350090E0B8}" name="TES5" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{9D8640EE-2549-45A3-98FD-B1C4A9FB399B}" name="TES7" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{BDF4F3C4-0105-422C-89EC-1C044F17D164}" name="Periodo" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{CD18CA5F-849B-477D-8347-AEC7C9F9C1A3}" name="Tasa_inter" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{7498D1B7-EF61-4ABC-A39A-C1ED050FE05F}" name="Consumo" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5D1D2915-40B4-4440-B8E5-EC65A8C1BDE2}" name="Comercial" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B3A56FF1-A864-41BA-9CEB-83FCFDC4BA73}" name="Hipotecario" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{40E2355E-A7FB-42F5-AF3D-31DBC2503E8C}" name="TES1" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{AE326550-1A7E-40C8-856D-05350090E0B8}" name="TES5" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{9D8640EE-2549-45A3-98FD-B1C4A9FB399B}" name="TES7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2463,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48954CB-18F3-40C5-B659-60FD6B4B1718}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2482,31 +2482,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -2997,28 +2997,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3592,28 +3592,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -4200,7 +4200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578166C7-2171-4399-9ED8-A01A918A2EFF}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -4213,28 +4213,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -4254,13 +4254,13 @@
         <v>22.243660260543674</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4280,13 +4280,13 @@
         <v>20.456100898719509</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -4306,13 +4306,13 @@
         <v>19.738011385114735</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>